<commit_message>
Fix error with SSA reported as being part of CAZ in the region description.
</commit_message>
<xml_diff>
--- a/ar6/registration_templates/IPCC_AR6_model_registration_REMIND-EDGET.xlsx
+++ b/ar6/registration_templates/IPCC_AR6_model_registration_REMIND-EDGET.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -3327,7 +3327,7 @@
     <t xml:space="preserve">CAZ</t>
   </si>
   <si>
-    <t xml:space="preserve">Canada, South Africa, NZ, Australia</t>
+    <t xml:space="preserve">Canada, NZ, Australia</t>
   </si>
   <si>
     <t xml:space="preserve">NEU</t>
@@ -3680,7 +3680,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="7" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="9" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -7022,14 +7022,14 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="24" width="10.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="24" width="24.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="24" width="24.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="24" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="24" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="24" width="26"/>
@@ -7274,7 +7274,7 @@
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="27.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="23.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="44.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="34.42"/>
@@ -11517,8 +11517,8 @@
   </sheetPr>
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Correctly unchecked conversion techs which are not used by REMIND by default.
</commit_message>
<xml_diff>
--- a/ar6/registration_templates/IPCC_AR6_model_registration_REMIND-EDGET.xlsx
+++ b/ar6/registration_templates/IPCC_AR6_model_registration_REMIND-EDGET.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -3210,10 +3210,10 @@
     <t xml:space="preserve">Coal to Liquids w/ CCS - Yes</t>
   </si>
   <si>
-    <t xml:space="preserve">Gas to Liquids w/o CCS - Yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gas to Liquids w/ CCS - Yes</t>
+    <t xml:space="preserve">Gas to Liquids w/o CCS - No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gas to Liquids w/ CCS - No</t>
   </si>
   <si>
     <t xml:space="preserve">Bioliquids w/o CCS - Yes</t>
@@ -3243,7 +3243,7 @@
     <t xml:space="preserve">Biomass to Gas w/o CCS - Yes</t>
   </si>
   <si>
-    <t xml:space="preserve">Biomass to Gas w/ CCS - Yes</t>
+    <t xml:space="preserve">Biomass to Gas w/ CCS - No</t>
   </si>
   <si>
     <t xml:space="preserve"># Heat Generation</t>
@@ -3264,7 +3264,7 @@
     <t xml:space="preserve">Geothermal Heat - Yes</t>
   </si>
   <si>
-    <t xml:space="preserve">Solarthermal Heat - Yes</t>
+    <t xml:space="preserve">Solarthermal Heat - No</t>
   </si>
   <si>
     <t xml:space="preserve">CHP (coupled heat and power) - Yes</t>
@@ -3680,7 +3680,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="9" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="12" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -7267,8 +7267,8 @@
   </sheetPr>
   <dimension ref="A1:MQ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V10" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y43" activeCellId="0" sqref="Y43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11517,7 +11517,7 @@
   </sheetPr>
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -12072,7 +12072,7 @@
   </sheetPr>
   <dimension ref="A1:J249"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A214" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A208" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update model registration templates for EDGET. Add templates for REMIND-MAGPIE and the old ENGAGE template.
</commit_message>
<xml_diff>
--- a/ar6/registration_templates/IPCC_AR6_model_registration_REMIND-EDGET.xlsx
+++ b/ar6/registration_templates/IPCC_AR6_model_registration_REMIND-EDGET.xlsx
@@ -3210,7 +3210,7 @@
     <t xml:space="preserve">Coal to Liquids w/ CCS - Yes</t>
   </si>
   <si>
-    <t xml:space="preserve">Gas to Liquids w/o CCS - No</t>
+    <t xml:space="preserve">Gas to Liquids w/o CCS - Yes</t>
   </si>
   <si>
     <t xml:space="preserve">Gas to Liquids w/ CCS - No</t>
@@ -3680,7 +3680,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="12" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -7268,7 +7268,7 @@
   <dimension ref="A1:MQ1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V10" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y43" activeCellId="0" sqref="Y43"/>
+      <selection pane="topLeft" activeCell="AA40" activeCellId="0" sqref="AA40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Changes to the coupled template: - changes as suggested in the mail by Isabelle from 9.6.:
Co-linkages -> Food Access - Yes, Water Availability - Yes, Biodiversity - Yes
Reforestation - Yes

Reiter Socio-economic Drivers:
Population Age Structure - Yes (exogenous)?

Reiter Consumer Heterogeneity and Behavior
"Agriculture - No" --> "Agriculture - Yes"
"Age - No"  --> "Age - Yes"
"Gender - No" --> "Gender - Yes"

Reiter Resource Use
Statt bisher "Land - No" --> "Land -  Yes (Process Model)"

Reiter Greenhouse Gas Emissions
"CO2 Land Use - Yes (exogenous baseline & controlled)" --> Yes (endogenous & controlled)

Changes to the EDGET template:
- added missing model names.
</commit_message>
<xml_diff>
--- a/ar6/registration_templates/IPCC_AR6_model_registration_REMIND-EDGET.xlsx
+++ b/ar6/registration_templates/IPCC_AR6_model_registration_REMIND-EDGET.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -2072,7 +2072,7 @@
     <t xml:space="preserve">yes </t>
   </si>
   <si>
-    <t xml:space="preserve">REMIND-EDGET 2.1</t>
+    <t xml:space="preserve">REMIND-Transport 2.1</t>
   </si>
   <si>
     <t xml:space="preserve">luderer</t>
@@ -7048,7 +7048,7 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7292,8 +7292,8 @@
   </sheetPr>
   <dimension ref="A1:MQ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AN1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AO2" activeCellId="0" sqref="AO2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11549,7 +11549,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11723,7 +11723,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12103,7 +12103,7 @@
   </sheetPr>
   <dimension ref="A1:J249"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A208" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A208" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
     </sheetView>
   </sheetViews>

</xml_diff>